<commit_message>
added analysis buttons in agv_simulation
</commit_message>
<xml_diff>
--- a/MATLAB/results_sensitivity.xlsx
+++ b/MATLAB/results_sensitivity.xlsx
@@ -12,13 +12,13 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" xr2:uid="{B799F073-4E72-4FDF-92A5-C2B15FC73B59}"/>
   </bookViews>
   <sheets>
-    <sheet name="Logic" sheetId="1" r:id="rId1"/>
+    <sheet name="Data" sheetId="1" r:id="rId1"/>
     <sheet name="Sensitivity" sheetId="4" r:id="rId2"/>
     <sheet name="Results" sheetId="3" r:id="rId3"/>
     <sheet name="Test Cases" sheetId="2" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="AGV_Params">Logic!$H$2:$L$12</definedName>
+    <definedName name="AGV_Params">Data!$H$2:$L$12</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -310,7 +310,7 @@
                   <c:v>-2.4095618164513E-4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-4.5083478023659473E-4</c:v>
+                  <c:v>-2.0987859859146474E-4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -740,7 +740,7 @@
                   <c:v>-2.4095618164513E-4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-4.5083478023659473E-4</c:v>
+                  <c:v>-2.0987859859146474E-4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3114,7 +3114,7 @@
       </c>
       <c r="B6">
         <f>Results!Q11</f>
-        <v>2.4965218115638031E-2</v>
+        <v>2.4724261933992901E-2</v>
       </c>
       <c r="C6">
         <f>Results!$Q$2</f>
@@ -3129,7 +3129,7 @@
       </c>
       <c r="G6">
         <f>C6-B6</f>
-        <v>-4.5083478023659473E-4</v>
+        <v>-2.0987859859146474E-4</v>
       </c>
       <c r="H6">
         <f>C6-D6</f>
@@ -3147,7 +3147,7 @@
   <dimension ref="A1:R12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:R1"/>
+      <selection activeCell="A2" sqref="A2:R12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3726,7 +3726,7 @@
         <v>16</v>
       </c>
       <c r="E11">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F11">
         <v>1</v>
@@ -3762,7 +3762,7 @@
         <v>550</v>
       </c>
       <c r="Q11">
-        <v>2.4965218115638031E-2</v>
+        <v>2.4724261933992901E-2</v>
       </c>
       <c r="R11">
         <v>0.75</v>
@@ -3891,23 +3891,23 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2">
-        <f>Logic!H2</f>
+        <f>Data!H2</f>
         <v>5.4</v>
       </c>
       <c r="B2">
-        <f>Logic!I2</f>
+        <f>Data!I2</f>
         <v>11</v>
       </c>
       <c r="C2">
-        <f>Logic!J2</f>
+        <f>Data!J2</f>
         <v>12</v>
       </c>
       <c r="D2">
-        <f>Logic!K2</f>
+        <f>Data!K2</f>
         <v>16</v>
       </c>
       <c r="E2">
-        <f>Logic!L2</f>
+        <f>Data!L2</f>
         <v>17</v>
       </c>
       <c r="F2">
@@ -3946,23 +3946,23 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3">
-        <f>Logic!H3</f>
+        <f>Data!H3</f>
         <v>4.9000000000000004</v>
       </c>
       <c r="B3">
-        <f>Logic!I3</f>
+        <f>Data!I3</f>
         <v>11</v>
       </c>
       <c r="C3">
-        <f>Logic!J3</f>
+        <f>Data!J3</f>
         <v>12</v>
       </c>
       <c r="D3">
-        <f>Logic!K3</f>
+        <f>Data!K3</f>
         <v>16</v>
       </c>
       <c r="E3">
-        <f>Logic!L3</f>
+        <f>Data!L3</f>
         <v>17</v>
       </c>
       <c r="F3">
@@ -4001,23 +4001,23 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f>Logic!H4</f>
+        <f>Data!H4</f>
         <v>5.9</v>
       </c>
       <c r="B4">
-        <f>Logic!I4</f>
+        <f>Data!I4</f>
         <v>11</v>
       </c>
       <c r="C4">
-        <f>Logic!J4</f>
+        <f>Data!J4</f>
         <v>12</v>
       </c>
       <c r="D4">
-        <f>Logic!K4</f>
+        <f>Data!K4</f>
         <v>16</v>
       </c>
       <c r="E4">
-        <f>Logic!L4</f>
+        <f>Data!L4</f>
         <v>17</v>
       </c>
       <c r="F4">
@@ -4056,23 +4056,23 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5">
-        <f>Logic!H5</f>
+        <f>Data!H5</f>
         <v>5.4</v>
       </c>
       <c r="B5">
-        <f>Logic!I5</f>
+        <f>Data!I5</f>
         <v>10</v>
       </c>
       <c r="C5">
-        <f>Logic!J5</f>
+        <f>Data!J5</f>
         <v>12</v>
       </c>
       <c r="D5">
-        <f>Logic!K5</f>
+        <f>Data!K5</f>
         <v>16</v>
       </c>
       <c r="E5">
-        <f>Logic!L5</f>
+        <f>Data!L5</f>
         <v>17</v>
       </c>
       <c r="F5">
@@ -4111,23 +4111,23 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6">
-        <f>Logic!H6</f>
+        <f>Data!H6</f>
         <v>5.4</v>
       </c>
       <c r="B6">
-        <f>Logic!I6</f>
+        <f>Data!I6</f>
         <v>12</v>
       </c>
       <c r="C6">
-        <f>Logic!J6</f>
+        <f>Data!J6</f>
         <v>12</v>
       </c>
       <c r="D6">
-        <f>Logic!K6</f>
+        <f>Data!K6</f>
         <v>16</v>
       </c>
       <c r="E6">
-        <f>Logic!L6</f>
+        <f>Data!L6</f>
         <v>17</v>
       </c>
       <c r="F6">
@@ -4166,23 +4166,23 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7">
-        <f>Logic!H7</f>
+        <f>Data!H7</f>
         <v>5.4</v>
       </c>
       <c r="B7">
-        <f>Logic!I7</f>
+        <f>Data!I7</f>
         <v>11</v>
       </c>
       <c r="C7">
-        <f>Logic!J7</f>
+        <f>Data!J7</f>
         <v>11</v>
       </c>
       <c r="D7">
-        <f>Logic!K7</f>
+        <f>Data!K7</f>
         <v>16</v>
       </c>
       <c r="E7">
-        <f>Logic!L7</f>
+        <f>Data!L7</f>
         <v>17</v>
       </c>
       <c r="F7">
@@ -4221,23 +4221,23 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8">
-        <f>Logic!H8</f>
+        <f>Data!H8</f>
         <v>5.4</v>
       </c>
       <c r="B8">
-        <f>Logic!I8</f>
+        <f>Data!I8</f>
         <v>11</v>
       </c>
       <c r="C8">
-        <f>Logic!J8</f>
+        <f>Data!J8</f>
         <v>13</v>
       </c>
       <c r="D8">
-        <f>Logic!K8</f>
+        <f>Data!K8</f>
         <v>16</v>
       </c>
       <c r="E8">
-        <f>Logic!L8</f>
+        <f>Data!L8</f>
         <v>17</v>
       </c>
       <c r="F8">
@@ -4276,23 +4276,23 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9">
-        <f>Logic!H9</f>
+        <f>Data!H9</f>
         <v>5.4</v>
       </c>
       <c r="B9">
-        <f>Logic!I9</f>
+        <f>Data!I9</f>
         <v>11</v>
       </c>
       <c r="C9">
-        <f>Logic!J9</f>
+        <f>Data!J9</f>
         <v>12</v>
       </c>
       <c r="D9">
-        <f>Logic!K9</f>
+        <f>Data!K9</f>
         <v>15</v>
       </c>
       <c r="E9">
-        <f>Logic!L9</f>
+        <f>Data!L9</f>
         <v>17</v>
       </c>
       <c r="F9">
@@ -4331,23 +4331,23 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10">
-        <f>Logic!H10</f>
+        <f>Data!H10</f>
         <v>5.4</v>
       </c>
       <c r="B10">
-        <f>Logic!I10</f>
+        <f>Data!I10</f>
         <v>11</v>
       </c>
       <c r="C10">
-        <f>Logic!J10</f>
+        <f>Data!J10</f>
         <v>12</v>
       </c>
       <c r="D10">
-        <f>Logic!K10</f>
+        <f>Data!K10</f>
         <v>17</v>
       </c>
       <c r="E10">
-        <f>Logic!L10</f>
+        <f>Data!L10</f>
         <v>17</v>
       </c>
       <c r="F10">
@@ -4386,23 +4386,23 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11">
-        <f>Logic!H11</f>
+        <f>Data!H11</f>
         <v>5.4</v>
       </c>
       <c r="B11">
-        <f>Logic!I11</f>
+        <f>Data!I11</f>
         <v>11</v>
       </c>
       <c r="C11">
-        <f>Logic!J11</f>
+        <f>Data!J11</f>
         <v>12</v>
       </c>
       <c r="D11">
-        <f>Logic!K11</f>
+        <f>Data!K11</f>
         <v>16</v>
       </c>
       <c r="E11">
-        <f>Logic!L11</f>
+        <f>Data!L11</f>
         <v>16</v>
       </c>
       <c r="F11">
@@ -4441,23 +4441,23 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12">
-        <f>Logic!H12</f>
+        <f>Data!H12</f>
         <v>5.4</v>
       </c>
       <c r="B12">
-        <f>Logic!I12</f>
+        <f>Data!I12</f>
         <v>11</v>
       </c>
       <c r="C12">
-        <f>Logic!J12</f>
+        <f>Data!J12</f>
         <v>12</v>
       </c>
       <c r="D12">
-        <f>Logic!K12</f>
+        <f>Data!K12</f>
         <v>16</v>
       </c>
       <c r="E12">
-        <f>Logic!L12</f>
+        <f>Data!L12</f>
         <v>18</v>
       </c>
       <c r="F12">

</xml_diff>

<commit_message>
open excel file after analysis is performed
</commit_message>
<xml_diff>
--- a/MATLAB/results_sensitivity.xlsx
+++ b/MATLAB/results_sensitivity.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" xr2:uid="{B799F073-4E72-4FDF-92A5-C2B15FC73B59}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="2" xr2:uid="{B799F073-4E72-4FDF-92A5-C2B15FC73B59}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -2433,7 +2433,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAD585F9-90CC-4715-96E5-A771C095B98B}">
   <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
@@ -3146,7 +3146,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9C33499-6AA4-459A-9B84-2EBC527BBE1E}">
   <dimension ref="A1:R12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:R12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
open correct worksheet in excel
</commit_message>
<xml_diff>
--- a/MATLAB/results_sensitivity.xlsx
+++ b/MATLAB/results_sensitivity.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="2" xr2:uid="{B799F073-4E72-4FDF-92A5-C2B15FC73B59}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" xr2:uid="{B799F073-4E72-4FDF-92A5-C2B15FC73B59}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -2433,8 +2433,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAD585F9-90CC-4715-96E5-A771C095B98B}">
   <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3146,7 +3146,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9C33499-6AA4-459A-9B84-2EBC527BBE1E}">
   <dimension ref="A1:R12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:R12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added tradeoff and Sensitivity analysis and elements to Papyrus model
</commit_message>
<xml_diff>
--- a/MATLAB/results_sensitivity.xlsx
+++ b/MATLAB/results_sensitivity.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Samvrit\Box Sync\ENSE 623 - System Verification\Project\MATLAB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kersa\Desktop\agv\MATLAB\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" xr2:uid="{B799F073-4E72-4FDF-92A5-C2B15FC73B59}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7536"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
   <definedNames>
     <definedName name="AGV_Params">Data!$H$2:$L$12</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -101,7 +101,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2430,16 +2430,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAD585F9-90CC-4715-96E5-A771C095B98B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -2474,7 +2474,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>20</v>
       </c>
@@ -2511,7 +2511,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>21</v>
       </c>
@@ -2548,7 +2548,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>19</v>
       </c>
@@ -2585,7 +2585,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>20</v>
       </c>
@@ -2622,7 +2622,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>20</v>
       </c>
@@ -2659,7 +2659,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>20</v>
       </c>
@@ -2696,7 +2696,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>20</v>
       </c>
@@ -2733,7 +2733,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>20</v>
       </c>
@@ -2770,7 +2770,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>20</v>
       </c>
@@ -2807,7 +2807,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>20</v>
       </c>
@@ -2844,7 +2844,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>20</v>
       </c>
@@ -2881,7 +2881,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D15" s="1"/>
       <c r="E15" s="1" t="s">
         <v>20</v>
@@ -2893,7 +2893,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D16" s="1" t="s">
         <v>0</v>
       </c>
@@ -2907,7 +2907,7 @@
         <v>5.9</v>
       </c>
     </row>
-    <row r="17" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D17" s="1" t="s">
         <v>1</v>
       </c>
@@ -2921,7 +2921,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D18" s="1" t="s">
         <v>2</v>
       </c>
@@ -2935,7 +2935,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D19" s="1" t="s">
         <v>3</v>
       </c>
@@ -2949,7 +2949,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D20" s="1" t="s">
         <v>4</v>
       </c>
@@ -2970,16 +2970,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF692D14-A8A6-4E78-AAB0-1AC29F8DB9FA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>21</v>
       </c>
@@ -2996,7 +2996,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -3024,7 +3024,7 @@
         <v>4.6373217819716678E-4</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -3052,7 +3052,7 @@
         <v>4.74450977324542E-4</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -3080,7 +3080,7 @@
         <v>3.9124622457956115E-4</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -3108,7 +3108,7 @@
         <v>2.098785985914578E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -3143,16 +3143,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9C33499-6AA4-459A-9B84-2EBC527BBE1E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:R12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3208,7 +3208,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>5.4</v>
       </c>
@@ -3264,7 +3264,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>4.9000000000000004</v>
       </c>
@@ -3320,7 +3320,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>5.9</v>
       </c>
@@ -3376,7 +3376,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>5.4</v>
       </c>
@@ -3432,7 +3432,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5.4</v>
       </c>
@@ -3488,7 +3488,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5.4</v>
       </c>
@@ -3544,7 +3544,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>5.4</v>
       </c>
@@ -3600,7 +3600,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>5.4</v>
       </c>
@@ -3656,7 +3656,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>5.4</v>
       </c>
@@ -3712,7 +3712,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>5.4</v>
       </c>
@@ -3768,7 +3768,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>5.4</v>
       </c>
@@ -3830,16 +3830,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DA3DE50-8D11-4121-8681-2B57E3545045}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3889,7 +3889,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2">
         <f>Data!H2</f>
         <v>5.4</v>
@@ -3944,7 +3944,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3">
         <f>Data!H3</f>
         <v>4.9000000000000004</v>
@@ -3999,7 +3999,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4">
         <f>Data!H4</f>
         <v>5.9</v>
@@ -4054,7 +4054,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>Data!H5</f>
         <v>5.4</v>
@@ -4109,7 +4109,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6">
         <f>Data!H6</f>
         <v>5.4</v>
@@ -4164,7 +4164,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7">
         <f>Data!H7</f>
         <v>5.4</v>
@@ -4219,7 +4219,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8">
         <f>Data!H8</f>
         <v>5.4</v>
@@ -4274,7 +4274,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9">
         <f>Data!H9</f>
         <v>5.4</v>
@@ -4329,7 +4329,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10">
         <f>Data!H10</f>
         <v>5.4</v>
@@ -4384,7 +4384,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11">
         <f>Data!H11</f>
         <v>5.4</v>
@@ -4439,7 +4439,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12">
         <f>Data!H12</f>
         <v>5.4</v>

</xml_diff>